<commit_message>
Bugfix: German Umlaute in Month name, dirty
Specifying Ã¤as \\"{a} is not clean.
Problems: Maerz is not passed to latex template in uft-8 but different
encoding
</commit_message>
<xml_diff>
--- a/02_logbook.xlsx
+++ b/02_logbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t xml:space="preserve">car</t>
   </si>
@@ -61,8 +61,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="HH:MM"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="hh:mm"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -136,7 +136,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -158,17 +158,21 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -178,18 +182,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.0714285714286"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.07"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -216,10 +220,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -228,7 +232,7 @@
       <c r="D2" s="2" t="n">
         <v>0.625</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="6" t="n">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="n">
@@ -239,10 +243,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -251,7 +255,7 @@
       <c r="D3" s="2" t="n">
         <v>0.625</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="6" t="n">
         <v>20</v>
       </c>
       <c r="F3" s="1" t="n">
@@ -262,10 +266,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -274,7 +278,7 @@
       <c r="D4" s="2" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="6" t="n">
         <v>30</v>
       </c>
       <c r="F4" s="1" t="n">
@@ -285,10 +289,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -297,7 +301,7 @@
       <c r="D5" s="2" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="6" t="n">
         <v>40</v>
       </c>
       <c r="F5" s="1" t="n">
@@ -308,10 +312,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -320,20 +324,112 @@
       <c r="D6" s="2" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="6" t="n">
         <v>50</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>36923</v>
       </c>
       <c r="G6" s="2" t="n">
+        <v>0.541666666666667</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>36951</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>36951</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0.708333333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>36952</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>36952</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0.708333333333333</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>36955</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>36955</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0.541666666666667</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>36951</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>36951</v>
+      </c>
+      <c r="G10" s="2" t="n">
         <v>0.541666666666667</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>